<commit_message>
Fixed baseline geom and mesh quality
</commit_message>
<xml_diff>
--- a/literature/wing_parameters.xlsx
+++ b/literature/wing_parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/296575b52adf77b6/Desktop/transonic_wing_analysis/geometry/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/296575b52adf77b6/Documents/Portfolio Projects/transonic_wing_analysis/literature/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{5B5EF574-0347-44C0-A558-CC9C74A56790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{292F4E3B-42CB-4416-9EEB-DF9D602710C6}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{5B5EF574-0347-44C0-A558-CC9C74A56790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5DDF07B-3DE2-4EF2-A031-ADA52D232010}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="0" windowWidth="9600" windowHeight="10800" xr2:uid="{22F203A8-2BA3-41EA-96B1-6872713AE8B3}"/>
+    <workbookView xWindow="1900" yWindow="0" windowWidth="12300" windowHeight="10800" xr2:uid="{22F203A8-2BA3-41EA-96B1-6872713AE8B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,6 +78,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{6E65E993-0E92-49A7-99B8-A9BE26A7EF77}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Shreyans Kinattumkara:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+in openVSP, 2.8deg roughly matches the planform shape from spec sheet</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -156,7 +180,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -208,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -216,10 +240,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -539,12 +560,12 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.90625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.90625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.90625" style="2" customWidth="1"/>
     <col min="3" max="3" width="5.1796875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="44.81640625" style="2" bestFit="1" customWidth="1"/>
@@ -566,7 +587,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2">
@@ -580,7 +601,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2">
@@ -594,7 +615,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="3">
@@ -608,7 +629,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -619,7 +640,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="2">
@@ -633,7 +654,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="2">
@@ -647,7 +668,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="2">
@@ -661,7 +682,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="2">

</xml_diff>